<commit_message>
Modify +/-15V Power On and Power Off logical
@shJoshDing
+15V and -15V power on/off have different GPIO status;
</commit_message>
<xml_diff>
--- a/Hardware Docs/SDP-B GPIO.xlsx
+++ b/Hardware Docs/SDP-B GPIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Signal Define" sheetId="1" r:id="rId1"/>
@@ -1200,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1626,7 @@
         <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>